<commit_message>
add luggage capacity graph
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-20" windowWidth="25440" windowHeight="13320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten CHF" sheetId="2" r:id="rId1"/>
@@ -13,8 +13,9 @@
     <sheet name="Drehmoment nach Getriebe" sheetId="4" r:id="rId4"/>
     <sheet name="Skalen m vs. km" sheetId="3" r:id="rId5"/>
     <sheet name="Skala mph_kph" sheetId="6" r:id="rId6"/>
+    <sheet name="Kofferraumvolumen" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="47">
   <si>
     <t>|</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -160,19 +161,38 @@
   <si>
     <t>Verbrenner</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Volvo XC70</t>
+  </si>
+  <si>
+    <t>Kofferraum (Sitze oben)</t>
+  </si>
+  <si>
+    <t>Audi A6 Avant</t>
+  </si>
+  <si>
+    <t>Front Kofferraum</t>
+  </si>
+  <si>
+    <t>zusätzlicher Kofferraum (Sitze runter klappen)</t>
+  </si>
+  <si>
+    <t>BMW 5er Touring</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0&quot;min&quot;"/>
     <numFmt numFmtId="165" formatCode="_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="0\ &quot;Nm&quot;"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="0\ &quot;L&quot;"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -197,6 +217,11 @@
     <font>
       <sz val="9"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -230,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -268,12 +293,14 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
@@ -299,8 +326,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -308,14 +344,15 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.167250166274058"/>
-          <c:y val="0.0514005540974045"/>
-          <c:w val="0.410538634625276"/>
-          <c:h val="0.832619568387285"/>
+          <c:y val="5.1400554097404502E-2"/>
+          <c:w val="0.41053863462527601"/>
+          <c:h val="0.83261956838728501"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -353,12 +390,18 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
             <c:separator>
 </c:separator>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -378,13 +421,13 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>45000.0</c:v>
+                  <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72400.0</c:v>
+                  <c:v>72400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -417,9 +460,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-          </c:dPt>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten CHF'!$B$1:$C$1</c:f>
@@ -438,13 +479,13 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1800.0</c:v>
+                  <c:v>1800</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -481,6 +522,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten CHF'!$B$1:$C$1</c:f>
@@ -499,13 +541,13 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2400.0</c:v>
+                  <c:v>2400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -549,6 +591,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten CHF'!$B$1:$C$1</c:f>
@@ -567,13 +610,13 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>20160.0</c:v>
+                  <c:v>20160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7360.0</c:v>
+                  <c:v>7360</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -618,6 +661,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten CHF'!$B$1:$C$1</c:f>
@@ -636,13 +680,13 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16000.0</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12000.0</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -686,6 +730,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten CHF'!$B$1:$C$1</c:f>
@@ -704,47 +749,61 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$7:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>10400.0</c:v>
+                  <c:v>10400</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4800.0</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="589279672"/>
-        <c:axId val="589282728"/>
+        <c:axId val="53900800"/>
+        <c:axId val="53902336"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="589279672"/>
+        <c:axId val="53900800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589282728"/>
+        <c:crossAx val="53902336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="589282728"/>
+        <c:axId val="53902336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_ [$Fr.-807]\ * #\'##0.00_ ;_ [$Fr.-807]\ * \-#\'##0.00_ ;_ [$Fr.-807]\ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:numFmt formatCode="_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589279672"/>
+        <c:crossAx val="53900800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -755,15 +814,17 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.60741842521149"/>
+          <c:x val="0.60741842521149003"/>
           <c:y val="0.150858486439195"/>
-          <c:w val="0.337636009574921"/>
-          <c:h val="0.504594352308382"/>
+          <c:w val="0.33763600957492101"/>
+          <c:h val="0.50459435230838201"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
     <a:bodyPr/>
@@ -781,7 +842,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -791,8 +852,17 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -800,14 +870,15 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.167250166274058"/>
-          <c:y val="0.0514005540974045"/>
-          <c:w val="0.410538634625276"/>
-          <c:h val="0.832619568387285"/>
+          <c:y val="5.1400554097404502E-2"/>
+          <c:w val="0.41053863462527601"/>
+          <c:h val="0.83261956838728501"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -845,12 +916,18 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
             <c:showSerName val="1"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
             <c:separator>
 </c:separator>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -870,13 +947,13 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\'##0.00\ [$€-407]_-;\-* #\'##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>29000.0</c:v>
+                  <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65300.0</c:v>
+                  <c:v>65300</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -909,9 +986,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-          </c:dPt>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten EUR'!$B$1:$C$1</c:f>
@@ -933,10 +1008,10 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>2160.0</c:v>
+                  <c:v>2160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -973,6 +1048,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten EUR'!$B$1:$C$1</c:f>
@@ -994,10 +1070,10 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14560.0</c:v>
+                  <c:v>14560</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6256.000000000001</c:v>
+                  <c:v>6256.0000000000009</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,6 +1117,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten EUR'!$B$1:$C$1</c:f>
@@ -1062,10 +1139,10 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>16000.0</c:v>
+                  <c:v>16000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12000.0</c:v>
+                  <c:v>12000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1110,6 +1187,7 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Kosten EUR'!$B$1:$C$1</c:f>
@@ -1131,44 +1209,58 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>7200.0</c:v>
+                  <c:v>7200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4800.0</c:v>
+                  <c:v>4800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="589143752"/>
-        <c:axId val="595225032"/>
+        <c:axId val="212183680"/>
+        <c:axId val="212197760"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="589143752"/>
+        <c:axId val="212183680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595225032"/>
+        <c:crossAx val="212197760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="595225032"/>
+        <c:axId val="212197760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_-* #\'##0.00\ [$€-407]_-;\-* #\'##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589143752"/>
+        <c:crossAx val="212183680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1179,15 +1271,17 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.60741842521149"/>
+          <c:x val="0.60741842521149003"/>
           <c:y val="0.150858486439195"/>
-          <c:w val="0.337636009574921"/>
-          <c:h val="0.504594352308382"/>
+          <c:w val="0.33763600957492101"/>
+          <c:h val="0.50459435230838201"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:txPr>
     <a:bodyPr/>
@@ -1205,7 +1299,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1215,7 +1309,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="18"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1225,14 +1327,15 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.153526235525938"/>
-          <c:y val="0.100831005137107"/>
-          <c:w val="0.813371915035585"/>
-          <c:h val="0.641503811077403"/>
+          <c:y val="0.10083100513710699"/>
+          <c:w val="0.81337191503558504"/>
+          <c:h val="0.64150381107740295"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1270,38 +1373,60 @@
               </a:solidFill>
             </a:ln>
           </c:spPr>
+          <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.000463787585285939"/>
-                  <c:y val="0.00123592164794603"/>
+                  <c:x val="-4.6378758528593897E-4"/>
+                  <c:y val="1.23592164794603E-3"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
                   <c:x val="-1.81734947254672E-7"/>
-                  <c:y val="-0.0144310802288519"/>
+                  <c:y val="-1.44310802288519E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0"/>
-                  <c:y val="-0.0240518003814199"/>
+                  <c:x val="0"/>
+                  <c:y val="-2.4051800381419901E-2"/>
                 </c:manualLayout>
               </c:layout>
+              <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
             </c:dLbl>
+            <c:showLegendKey val="0"/>
             <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
@@ -1327,10 +1452,12 @@
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>zuhause _x000d_(230V, 10A)</c:v>
+                    <c:v>zuhause 
+(230V, 10A)</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>zuhause_x000d_(230V, 16A)</c:v>
+                    <c:v>zuhause
+(230V, 16A)</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>zuhause (3Phasen, 400V)</c:v>
@@ -1352,64 +1479,79 @@
                 <c:formatCode>0"min"</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>600.0</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>380.0</c:v>
+                  <c:v>380</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>120.0</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>60.0</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>12.0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="589168600"/>
-        <c:axId val="589171656"/>
+        <c:axId val="226652928"/>
+        <c:axId val="226654464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="589168600"/>
+        <c:axId val="226652928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589171656"/>
+        <c:crossAx val="226654464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="589171656"/>
+        <c:axId val="226654464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="600.0"/>
+          <c:max val="600"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0&quot;min&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="589168600"/>
+        <c:crossAx val="226652928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="50.0"/>
+        <c:majorUnit val="50"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1419,16 +1561,27 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="2"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$5:$D$5</c:f>
@@ -1450,54 +1603,70 @@
                 <c:formatCode>0\ "Nm"</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>550.0</c:v>
+                  <c:v>550</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>450.0</c:v>
+                  <c:v>450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="595143848"/>
-        <c:axId val="595136600"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="53868416"/>
+        <c:axId val="53869952"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="595143848"/>
+        <c:axId val="53868416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595136600"/>
+        <c:crossAx val="53869952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="595136600"/>
+        <c:axId val="53869952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="1000.0"/>
+          <c:max val="1000"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0\ &quot;Nm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595143848"/>
+        <c:crossAx val="53868416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="500.0"/>
+        <c:majorUnit val="500"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1507,13 +1676,23 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="3"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="103"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="3"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1528,6 +1707,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1546,7 +1726,7 @@
                 <c:formatCode>0\ "Nm"</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2294.05</c:v>
+                  <c:v>2294.0500000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1566,6 +1746,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1584,7 +1765,7 @@
                 <c:formatCode>0\ "Nm"</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1287.0</c:v>
+                  <c:v>1287</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1604,6 +1785,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1642,6 +1824,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1680,6 +1863,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1718,6 +1902,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
               <c:f>'Drehmoment nach Getriebe'!$C$7</c:f>
@@ -1736,39 +1921,53 @@
                 <c:formatCode>0\ "Nm"</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>380.05</c:v>
+                  <c:v>380.04999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="595332728"/>
-        <c:axId val="595335784"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="226683520"/>
+        <c:axId val="226496896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="595332728"/>
+        <c:axId val="226683520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595335784"/>
+        <c:crossAx val="226496896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="595335784"/>
+        <c:axId val="226496896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="5000.0"/>
+          <c:max val="5000"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0\ &quot;Nm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:txPr>
           <a:bodyPr/>
@@ -1780,7 +1979,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="595332728"/>
+        <c:crossAx val="226683520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1791,10 +1990,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.56396706631896"/>
+          <c:x val="0.56396706631895999"/>
           <c:y val="0.153469896848624"/>
           <c:w val="0.170799863708198"/>
-          <c:h val="0.572140779216214"/>
+          <c:h val="0.57214077921621398"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -1811,10 +2010,11 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1824,7 +2024,15 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
-  <c:style val="6"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="106"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="6"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
@@ -1833,15 +2041,16 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.047266738716484"/>
-          <c:y val="0.194328885972587"/>
-          <c:w val="0.653773492217216"/>
-          <c:h val="0.689691236512103"/>
+          <c:x val="4.7266738716484E-2"/>
+          <c:y val="0.19432888597258699"/>
+          <c:w val="0.65377349221721603"/>
+          <c:h val="0.68969123651210296"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
         <c:barDir val="bar"/>
         <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1856,6 +2065,7 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:invertIfNegative val="0"/>
           <c:val>
             <c:numRef>
               <c:f>'Drehmoment nach Getriebe'!$D$8</c:f>
@@ -1869,44 +2079,393 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
-        <c:axId val="595345784"/>
-        <c:axId val="595348840"/>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="226514432"/>
+        <c:axId val="226515968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="595345784"/>
+        <c:axId val="226514432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="1"/>
         <c:axPos val="l"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595348840"/>
+        <c:crossAx val="226515968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="595348840"/>
+        <c:axId val="226515968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0\ &quot;Nm&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="595345784"/>
+        <c:crossAx val="226514432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.787401575" l="0.7" r="0.7" t="0.787401575" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="139"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="39"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.9686891491124493E-2"/>
+          <c:y val="5.5243082574215077E-2"/>
+          <c:w val="0.5594411532893292"/>
+          <c:h val="0.59911663004968341"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Kofferraum (Sitze oben)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:alpha val="84000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$B$2:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Tesla Model S</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audi A6 Avant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BMW 5er Touring</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Volvo XC70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kofferraumvolumen!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "L"</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>744.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>485</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>zusätzlicher Kofferraum (Sitze runter klappen)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:alpha val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$B$2:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Tesla Model S</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audi A6 Avant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BMW 5er Touring</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Volvo XC70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kofferraumvolumen!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "L"</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>900.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1115</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1110</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1156</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Front Kofferraum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="tx2">
+                <a:lumMod val="50000"/>
+                <a:alpha val="72000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Kofferraumvolumen!$B$2:$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Tesla Model S</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Audi A6 Avant</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>BMW 5er Touring</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Volvo XC70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Kofferraumvolumen!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>0\ "L"</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>150.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="82"/>
+        <c:overlap val="100"/>
+        <c:axId val="227173888"/>
+        <c:axId val="227175424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="227173888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr rot="0" vert="horz"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="227175424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="227175424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0\ &quot;L&quot;" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="227173888"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8299668033399559E-2"/>
+          <c:y val="0.78289401687638582"/>
+          <c:w val="0.55818571647785897"/>
+          <c:h val="0.18312312849323237"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2106,6 +2665,41 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>1656503</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>87086</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>700064</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>65313</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2433,22 +3027,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>40</v>
       </c>
@@ -2456,7 +3050,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -2473,7 +3067,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2491,7 +3085,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -2509,7 +3103,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2528,7 +3122,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -2541,7 +3135,7 @@
         <v>12000</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -2560,7 +3154,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
         <v>95760</v>
@@ -2589,22 +3183,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="30.375" customWidth="1"/>
+    <col min="2" max="2" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="15.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="16" t="s">
         <v>39</v>
       </c>
@@ -2612,12 +3206,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="15">
-        <v>29000</v>
+        <v>48000</v>
       </c>
       <c r="C2" s="15">
         <v>65300</v>
@@ -2629,7 +3223,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2647,7 +3241,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>19</v>
       </c>
@@ -2666,7 +3260,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -2685,7 +3279,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2698,10 +3292,10 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <f>SUM(B2:B6)</f>
-        <v>68920</v>
+        <v>87920</v>
       </c>
       <c r="C7" s="15">
         <f>SUM(C2:C6)</f>
@@ -2714,7 +3308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D8">
         <v>23</v>
       </c>
@@ -2735,7 +3329,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A17:AB24"/>
   <sheetViews>
@@ -2743,28 +3337,28 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="4.140625" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="4.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.25" style="4" customWidth="1"/>
+    <col min="2" max="2" width="18.75" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="28" width="3.7109375" style="4" customWidth="1"/>
-    <col min="29" max="16384" width="4.140625" style="1"/>
+    <col min="5" max="28" width="3.75" style="4" customWidth="1"/>
+    <col min="29" max="16384" width="4.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D17" s="4">
         <f>75/4*60</f>
         <v>1125</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="D19" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="24">
+    <row r="20" spans="2:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="B20" s="14" t="s">
         <v>36</v>
       </c>
@@ -2775,7 +3369,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="24">
+    <row r="21" spans="2:4" ht="23.25" x14ac:dyDescent="0.2">
       <c r="B21" s="14" t="s">
         <v>33</v>
       </c>
@@ -2786,7 +3380,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>4</v>
       </c>
@@ -2797,7 +3391,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2808,7 +3402,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="4" t="s">
         <v>3</v>
       </c>
@@ -2833,7 +3427,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="B5:D13"/>
   <sheetViews>
@@ -2841,9 +3435,9 @@
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
         <v>25</v>
       </c>
@@ -2851,7 +3445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>32</v>
       </c>
@@ -2862,7 +3456,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>25</v>
       </c>
@@ -2870,7 +3464,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>26</v>
       </c>
@@ -2883,7 +3477,7 @@
         <v>4378.5</v>
       </c>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>27</v>
       </c>
@@ -2893,7 +3487,7 @@
       </c>
       <c r="D9" s="12"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>28</v>
       </c>
@@ -2903,7 +3497,7 @@
       </c>
       <c r="D10" s="12"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>29</v>
       </c>
@@ -2913,7 +3507,7 @@
       </c>
       <c r="D11" s="12"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>30</v>
       </c>
@@ -2923,7 +3517,7 @@
       </c>
       <c r="D12" s="12"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>31</v>
       </c>
@@ -2946,7 +3540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F20"/>
   <sheetViews>
@@ -2954,20 +3548,20 @@
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="7.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" style="7"/>
+    <col min="4" max="4" width="7.25" style="7" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="21" customHeight="1">
+    <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
       <c r="F1" s="8"/>
     </row>
-    <row r="2" spans="1:6" ht="21" customHeight="1">
+    <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>700</v>
       </c>
@@ -2975,7 +3569,7 @@
         <f>A2/1.6</f>
         <v>437.5</v>
       </c>
-      <c r="C2" s="17" t="s">
+      <c r="C2" s="19" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="9">
@@ -2986,7 +3580,7 @@
       </c>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="21" customHeight="1">
+    <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>650</v>
       </c>
@@ -2994,7 +3588,7 @@
         <f t="shared" ref="B3:B16" si="0">A3/1.6</f>
         <v>406.25</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="19"/>
       <c r="D3" s="9">
         <v>405</v>
       </c>
@@ -3003,7 +3597,7 @@
       </c>
       <c r="F3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="21" customHeight="1">
+    <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>600</v>
       </c>
@@ -3011,7 +3605,7 @@
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="C4" s="17"/>
+      <c r="C4" s="19"/>
       <c r="D4" s="9">
         <v>375</v>
       </c>
@@ -3020,7 +3614,7 @@
       </c>
       <c r="F4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="21" customHeight="1">
+    <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>550</v>
       </c>
@@ -3028,7 +3622,7 @@
         <f t="shared" si="0"/>
         <v>343.75</v>
       </c>
-      <c r="C5" s="17"/>
+      <c r="C5" s="19"/>
       <c r="D5" s="9">
         <v>345</v>
       </c>
@@ -3037,7 +3631,7 @@
       </c>
       <c r="F5" s="8"/>
     </row>
-    <row r="6" spans="1:6" ht="21" customHeight="1">
+    <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
@@ -3045,7 +3639,7 @@
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="C6" s="17"/>
+      <c r="C6" s="19"/>
       <c r="D6" s="9">
         <v>310</v>
       </c>
@@ -3054,7 +3648,7 @@
       </c>
       <c r="F6" s="8"/>
     </row>
-    <row r="7" spans="1:6" ht="21" customHeight="1">
+    <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>450</v>
       </c>
@@ -3062,7 +3656,7 @@
         <f t="shared" si="0"/>
         <v>281.25</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="19"/>
       <c r="D7" s="9">
         <v>280</v>
       </c>
@@ -3071,7 +3665,7 @@
       </c>
       <c r="F7" s="8"/>
     </row>
-    <row r="8" spans="1:6" ht="21" customHeight="1">
+    <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>400</v>
       </c>
@@ -3079,7 +3673,7 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C8" s="17"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="9">
         <v>250</v>
       </c>
@@ -3088,7 +3682,7 @@
       </c>
       <c r="F8" s="8"/>
     </row>
-    <row r="9" spans="1:6" ht="21" customHeight="1">
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>350</v>
       </c>
@@ -3096,7 +3690,7 @@
         <f t="shared" si="0"/>
         <v>218.75</v>
       </c>
-      <c r="C9" s="17"/>
+      <c r="C9" s="19"/>
       <c r="D9" s="9">
         <v>220</v>
       </c>
@@ -3105,7 +3699,7 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="10" spans="1:6" ht="21" customHeight="1">
+    <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>300</v>
       </c>
@@ -3113,7 +3707,7 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="C10" s="17"/>
+      <c r="C10" s="19"/>
       <c r="D10" s="9">
         <v>190</v>
       </c>
@@ -3122,7 +3716,7 @@
       </c>
       <c r="F10" s="8"/>
     </row>
-    <row r="11" spans="1:6" ht="21" customHeight="1">
+    <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>250</v>
       </c>
@@ -3130,7 +3724,7 @@
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C11" s="17"/>
+      <c r="C11" s="19"/>
       <c r="D11" s="9">
         <v>160</v>
       </c>
@@ -3139,7 +3733,7 @@
       </c>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:6" ht="21" customHeight="1">
+    <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
@@ -3147,7 +3741,7 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="19"/>
       <c r="D12" s="9">
         <v>125</v>
       </c>
@@ -3156,7 +3750,7 @@
       </c>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="21" customHeight="1">
+    <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>150</v>
       </c>
@@ -3164,7 +3758,7 @@
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="19"/>
       <c r="D13" s="9">
         <v>100</v>
       </c>
@@ -3173,7 +3767,7 @@
       </c>
       <c r="F13" s="8"/>
     </row>
-    <row r="14" spans="1:6" ht="21" customHeight="1">
+    <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -3181,7 +3775,7 @@
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C14" s="17"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="9">
         <v>65</v>
       </c>
@@ -3190,7 +3784,7 @@
       </c>
       <c r="F14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="21" customHeight="1">
+    <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>50</v>
       </c>
@@ -3198,7 +3792,7 @@
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C15" s="17"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="9">
         <v>30</v>
       </c>
@@ -3207,7 +3801,7 @@
       </c>
       <c r="F15" s="8"/>
     </row>
-    <row r="16" spans="1:6" ht="21" customHeight="1">
+    <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
@@ -3215,7 +3809,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="17"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="9">
         <v>0</v>
       </c>
@@ -3224,28 +3818,28 @@
       </c>
       <c r="F16" s="8"/>
     </row>
-    <row r="17" spans="2:6" ht="21" customHeight="1">
+    <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="8"/>
     </row>
-    <row r="18" spans="2:6" ht="21" customHeight="1">
+    <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="8"/>
     </row>
-    <row r="19" spans="2:6" ht="21" customHeight="1">
+    <row r="19" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="8"/>
     </row>
-    <row r="20" spans="2:6" ht="21" customHeight="1">
+    <row r="20" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
       <c r="D20" s="9"/>
@@ -3253,7 +3847,6 @@
       <c r="F20" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="C2:C16"/>
   </mergeCells>
@@ -3268,7 +3861,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AB7"/>
   <sheetViews>
@@ -3276,9 +3869,9 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="3.625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:28" s="1" customFormat="1">
+    <row r="1" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -3308,7 +3901,7 @@
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1">
+    <row r="2" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3390,7 +3983,7 @@
       </c>
       <c r="AB2" s="2"/>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="5" customHeight="1">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -3420,7 +4013,7 @@
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1">
+    <row r="4" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -3504,117 +4097,117 @@
       </c>
       <c r="AB4" s="2"/>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1">
+    <row r="5" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
-        <f>B4*1.60934</f>
+        <f t="shared" ref="B5:AA5" si="0">B4*1.60934</f>
         <v>0</v>
       </c>
       <c r="C5" s="3">
-        <f>C4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>8.0466999999999995</v>
       </c>
       <c r="D5" s="3">
-        <f>D4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>16.093399999999999</v>
       </c>
       <c r="E5" s="3">
-        <f>E4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>24.1401</v>
       </c>
       <c r="F5" s="3">
-        <f>F4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>32.186799999999998</v>
       </c>
       <c r="G5" s="3">
-        <f>G4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>40.233499999999999</v>
       </c>
       <c r="H5" s="3">
-        <f>H4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>48.280200000000001</v>
       </c>
       <c r="I5" s="3">
-        <f>I4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>56.326900000000002</v>
       </c>
       <c r="J5" s="3">
-        <f>J4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>64.373599999999996</v>
       </c>
       <c r="K5" s="3">
-        <f>K4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>72.420299999999997</v>
       </c>
       <c r="L5" s="3">
-        <f>L4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>80.466999999999999</v>
       </c>
       <c r="M5" s="3">
-        <f>M4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>88.5137</v>
       </c>
       <c r="N5" s="3">
-        <f>N4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>96.560400000000001</v>
       </c>
       <c r="O5" s="3">
-        <f>O4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>104.6071</v>
       </c>
       <c r="P5" s="3">
-        <f>P4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>112.6538</v>
       </c>
       <c r="Q5" s="3">
-        <f>Q4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>120.70050000000001</v>
       </c>
       <c r="R5" s="3">
-        <f>R4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>128.74719999999999</v>
       </c>
       <c r="S5" s="3">
-        <f>S4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>136.79390000000001</v>
       </c>
       <c r="T5" s="3">
-        <f>T4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>144.84059999999999</v>
       </c>
       <c r="U5" s="3">
-        <f>U4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>152.88730000000001</v>
       </c>
       <c r="V5" s="3">
-        <f>V4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>160.934</v>
       </c>
       <c r="W5" s="3">
-        <f>W4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>168.98070000000001</v>
       </c>
       <c r="X5" s="3">
-        <f>X4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>177.0274</v>
       </c>
       <c r="Y5" s="3">
-        <f>Y4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>185.07409999999999</v>
       </c>
       <c r="Z5" s="3">
-        <f>Z4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>193.1208</v>
       </c>
       <c r="AA5" s="3">
-        <f>AA4*1.60934</f>
+        <f t="shared" si="0"/>
         <v>201.16749999999999</v>
       </c>
       <c r="AB5" s="3"/>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1">
+    <row r="6" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3644,7 +4237,7 @@
       <c r="AA6" s="2"/>
       <c r="AB6" s="2"/>
     </row>
-    <row r="7" spans="1:28" s="1" customFormat="1">
+    <row r="7" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3675,7 +4268,6 @@
       <c r="AB7" s="2"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -3685,4 +4277,111 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr published="0"/>
+  <dimension ref="A2:E6"/>
+  <sheetViews>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="34.625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="16.125" customWidth="1"/>
+    <col min="4" max="4" width="16.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="17">
+        <v>744.7</v>
+      </c>
+      <c r="C3" s="17">
+        <v>565</v>
+      </c>
+      <c r="D3" s="17">
+        <v>560</v>
+      </c>
+      <c r="E3" s="17">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="17">
+        <f>B6-B3</f>
+        <v>900.5</v>
+      </c>
+      <c r="C4" s="17">
+        <f>C6-C3</f>
+        <v>1115</v>
+      </c>
+      <c r="D4" s="17">
+        <f>D6-D3</f>
+        <v>1110</v>
+      </c>
+      <c r="E4" s="17">
+        <f>E6-E3</f>
+        <v>1156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="17">
+        <v>150.1</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B6" s="17">
+        <v>1645.2</v>
+      </c>
+      <c r="C6" s="17">
+        <v>1680</v>
+      </c>
+      <c r="D6" s="17">
+        <v>1670</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1641</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
version 1.0, copyright note, more expensive power for EUR version
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten CHF" sheetId="2" r:id="rId1"/>
@@ -219,7 +219,7 @@
     <numFmt numFmtId="166" formatCode="0\ &quot;Nm&quot;"/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;L&quot;"/>
-    <numFmt numFmtId="170" formatCode="0.0\ &quot;sec&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.0\ &quot;sec&quot;"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -324,10 +324,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -336,6 +336,10 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFF5F9CF"/>
+      <color rgb="FFF2E47E"/>
+      <color rgb="FFF5D933"/>
+      <color rgb="FFEFDE5F"/>
       <color rgb="FFCAE8CF"/>
       <color rgb="FF7E1818"/>
       <color rgb="FFA8B5C4"/>
@@ -801,11 +805,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="53900800"/>
-        <c:axId val="53902336"/>
+        <c:axId val="235833216"/>
+        <c:axId val="235834752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53900800"/>
+        <c:axId val="235833216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53902336"/>
+        <c:crossAx val="235834752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -822,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53902336"/>
+        <c:axId val="235834752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53900800"/>
+        <c:crossAx val="235833216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,10 +981,10 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>48000</c:v>
+                  <c:v>50000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>65300</c:v>
@@ -1035,7 +1039,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2160</c:v>
@@ -1062,19 +1066,22 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="50000"/>
-                <a:lumOff val="50000"/>
-                <a:alpha val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:gradFill>
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:srgbClr val="F5D933">
+                    <a:alpha val="80000"/>
+                  </a:srgbClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:srgbClr val="F5F9CF"/>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
             <a:ln>
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:srgbClr val="C00000"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1097,13 +1104,13 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>14560</c:v>
+                  <c:v>21840</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6256.0000000000009</c:v>
+                  <c:v>15456</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1127,23 +1134,26 @@
             <a:gradFill>
               <a:gsLst>
                 <a:gs pos="0">
-                  <a:srgbClr val="FFC000">
-                    <a:alpha val="70000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="40000"/>
+                    <a:lumOff val="60000"/>
+                  </a:schemeClr>
                 </a:gs>
                 <a:gs pos="100000">
-                  <a:srgbClr val="FFFF00">
-                    <a:alpha val="38000"/>
-                  </a:srgbClr>
+                  <a:schemeClr val="tx2">
+                    <a:lumMod val="20000"/>
+                    <a:lumOff val="80000"/>
+                  </a:schemeClr>
                 </a:gs>
               </a:gsLst>
               <a:lin ang="5400000" scaled="0"/>
             </a:gradFill>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="FF0000">
+                <a:schemeClr val="tx2">
+                  <a:lumMod val="75000"/>
                   <a:alpha val="92000"/>
-                </a:srgbClr>
+                </a:schemeClr>
               </a:solidFill>
             </a:ln>
           </c:spPr>
@@ -1166,7 +1176,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>16000</c:v>
@@ -1236,7 +1246,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>7200</c:v>
@@ -1258,11 +1268,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="227453568"/>
-        <c:axId val="227467648"/>
+        <c:axId val="170026112"/>
+        <c:axId val="170027648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="227453568"/>
+        <c:axId val="170026112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1271,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227467648"/>
+        <c:crossAx val="170027648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1279,18 +1289,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="227467648"/>
+        <c:axId val="170027648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="227453568"/>
+        <c:crossAx val="170026112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1536,11 +1546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="241922816"/>
-        <c:axId val="241924352"/>
+        <c:axId val="170093568"/>
+        <c:axId val="170107648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="241922816"/>
+        <c:axId val="170093568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1549,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241924352"/>
+        <c:crossAx val="170107648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1557,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241924352"/>
+        <c:axId val="170107648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1569,7 +1579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241922816"/>
+        <c:crossAx val="170093568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1651,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="53868416"/>
-        <c:axId val="53869952"/>
+        <c:axId val="171774336"/>
+        <c:axId val="171775872"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="53868416"/>
+        <c:axId val="171774336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1664,7 +1674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53869952"/>
+        <c:crossAx val="171775872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1672,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="53869952"/>
+        <c:axId val="171775872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1684,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="53868416"/>
+        <c:crossAx val="171774336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1966,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="241953408"/>
-        <c:axId val="241766784"/>
+        <c:axId val="213435520"/>
+        <c:axId val="213437056"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="241953408"/>
+        <c:axId val="213435520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1979,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241766784"/>
+        <c:crossAx val="213437056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1987,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241766784"/>
+        <c:axId val="213437056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2009,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="241953408"/>
+        <c:crossAx val="213435520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2118,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="241773952"/>
-        <c:axId val="241792128"/>
+        <c:axId val="213444480"/>
+        <c:axId val="213446016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="241773952"/>
+        <c:axId val="213444480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2131,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241792128"/>
+        <c:crossAx val="213446016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2139,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241792128"/>
+        <c:axId val="213446016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2150,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241773952"/>
+        <c:crossAx val="213444480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2428,11 +2438,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="242441600"/>
-        <c:axId val="242447488"/>
+        <c:axId val="236066688"/>
+        <c:axId val="236068224"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="242441600"/>
+        <c:axId val="236066688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2451,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="242447488"/>
+        <c:crossAx val="236068224"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2459,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242447488"/>
+        <c:axId val="236068224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2470,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242441600"/>
+        <c:crossAx val="236066688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2726,11 +2736,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="76027392"/>
-        <c:axId val="76028928"/>
+        <c:axId val="236438272"/>
+        <c:axId val="236439808"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76027392"/>
+        <c:axId val="236438272"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2739,7 +2749,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76028928"/>
+        <c:crossAx val="236439808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2747,7 +2757,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76028928"/>
+        <c:axId val="236439808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2758,7 +2768,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76027392"/>
+        <c:crossAx val="236438272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3528,8 +3538,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3552,7 +3562,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="15">
-        <v>48000</v>
+        <v>50000</v>
       </c>
       <c r="C2" s="15">
         <v>65300</v>
@@ -3576,7 +3586,7 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="E3" t="s">
         <v>14</v>
@@ -3588,11 +3598,11 @@
       </c>
       <c r="B4" s="15">
         <f>D2*D3/100*D5*D4</f>
-        <v>14560</v>
+        <v>21840</v>
       </c>
       <c r="C4" s="15">
         <f>D2*D3*D7/100*D8</f>
-        <v>6256.0000000000009</v>
+        <v>15456</v>
       </c>
       <c r="D4">
         <v>1.3</v>
@@ -3636,14 +3646,14 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <f>SUM(B2:B6)</f>
-        <v>87920</v>
+        <v>97200</v>
       </c>
       <c r="C7" s="15">
         <f>SUM(C2:C6)</f>
-        <v>88356</v>
+        <v>97556</v>
       </c>
       <c r="D7">
-        <v>0.17</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>38</v>
@@ -3910,7 +3920,7 @@
         <f>A2/1.6</f>
         <v>437.5</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="9">
@@ -3929,7 +3939,7 @@
         <f t="shared" ref="B3:B16" si="0">A3/1.6</f>
         <v>406.25</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="9">
         <v>405</v>
       </c>
@@ -3946,7 +3956,7 @@
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="9">
         <v>375</v>
       </c>
@@ -3963,7 +3973,7 @@
         <f t="shared" si="0"/>
         <v>343.75</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="9">
         <v>345</v>
       </c>
@@ -3980,7 +3990,7 @@
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="C6" s="19"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="9">
         <v>310</v>
       </c>
@@ -3997,7 +4007,7 @@
         <f t="shared" si="0"/>
         <v>281.25</v>
       </c>
-      <c r="C7" s="19"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="9">
         <v>280</v>
       </c>
@@ -4014,7 +4024,7 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C8" s="19"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="9">
         <v>250</v>
       </c>
@@ -4031,7 +4041,7 @@
         <f t="shared" si="0"/>
         <v>218.75</v>
       </c>
-      <c r="C9" s="19"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="9">
         <v>220</v>
       </c>
@@ -4048,7 +4058,7 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="C10" s="19"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="9">
         <v>190</v>
       </c>
@@ -4065,7 +4075,7 @@
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C11" s="19"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="9">
         <v>160</v>
       </c>
@@ -4082,7 +4092,7 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C12" s="19"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="9">
         <v>125</v>
       </c>
@@ -4099,7 +4109,7 @@
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
-      <c r="C13" s="19"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="9">
         <v>100</v>
       </c>
@@ -4116,7 +4126,7 @@
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C14" s="19"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="9">
         <v>65</v>
       </c>
@@ -4133,7 +4143,7 @@
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="9">
         <v>30</v>
       </c>
@@ -4150,7 +4160,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="9">
         <v>0</v>
       </c>
@@ -4732,7 +4742,7 @@
   <sheetPr published="0"/>
   <dimension ref="A2:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -4774,28 +4784,28 @@
       <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="19">
         <v>5.6</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="19">
         <v>6.2</v>
       </c>
-      <c r="E3" s="20">
+      <c r="E3" s="19">
         <v>4.5</v>
       </c>
-      <c r="F3" s="20">
+      <c r="F3" s="19">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G3" s="20">
+      <c r="G3" s="19">
         <v>5.4</v>
       </c>
-      <c r="H3" s="20">
+      <c r="H3" s="19">
         <v>10.1</v>
       </c>
-      <c r="I3" s="20">
+      <c r="I3" s="19">
         <v>10.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
v1.1: updated energy costs for EUR edition
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -805,11 +805,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="235833216"/>
-        <c:axId val="235834752"/>
+        <c:axId val="80177024"/>
+        <c:axId val="80178560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="235833216"/>
+        <c:axId val="80177024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235834752"/>
+        <c:crossAx val="80178560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235834752"/>
+        <c:axId val="80178560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235833216"/>
+        <c:crossAx val="80177024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,7 +984,7 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>50000</c:v>
+                  <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>65300</c:v>
@@ -1039,7 +1039,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2160</c:v>
@@ -1107,10 +1107,10 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>21840</c:v>
+                  <c:v>23520</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15456</c:v>
+                  <c:v>12696</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1176,7 +1176,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>16000</c:v>
@@ -1246,7 +1246,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>7200</c:v>
@@ -1268,11 +1268,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="170026112"/>
-        <c:axId val="170027648"/>
+        <c:axId val="80264192"/>
+        <c:axId val="80278272"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170026112"/>
+        <c:axId val="80264192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170027648"/>
+        <c:crossAx val="80278272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1289,7 +1289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170027648"/>
+        <c:axId val="80278272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170026112"/>
+        <c:crossAx val="80264192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,11 +1546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="170093568"/>
-        <c:axId val="170107648"/>
+        <c:axId val="166757504"/>
+        <c:axId val="166759040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="170093568"/>
+        <c:axId val="166757504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170107648"/>
+        <c:crossAx val="166759040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="170107648"/>
+        <c:axId val="166759040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1579,7 +1579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="170093568"/>
+        <c:crossAx val="166757504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1661,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="171774336"/>
-        <c:axId val="171775872"/>
+        <c:axId val="181385472"/>
+        <c:axId val="181391360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="171774336"/>
+        <c:axId val="181385472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171775872"/>
+        <c:crossAx val="181391360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="171775872"/>
+        <c:axId val="181391360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1694,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171774336"/>
+        <c:crossAx val="181385472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1976,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213435520"/>
-        <c:axId val="213437056"/>
+        <c:axId val="181711616"/>
+        <c:axId val="181713152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213435520"/>
+        <c:axId val="181711616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213437056"/>
+        <c:crossAx val="181713152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213437056"/>
+        <c:axId val="181713152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2019,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="213435520"/>
+        <c:crossAx val="181711616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="213444480"/>
-        <c:axId val="213446016"/>
+        <c:axId val="181729152"/>
+        <c:axId val="181730688"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="213444480"/>
+        <c:axId val="181729152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213446016"/>
+        <c:crossAx val="181730688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="213446016"/>
+        <c:axId val="181730688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="213444480"/>
+        <c:crossAx val="181729152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,11 +2438,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="236066688"/>
-        <c:axId val="236068224"/>
+        <c:axId val="181827456"/>
+        <c:axId val="181828992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="236066688"/>
+        <c:axId val="181827456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="236068224"/>
+        <c:crossAx val="181828992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2469,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236068224"/>
+        <c:axId val="181828992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236066688"/>
+        <c:crossAx val="181827456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2541,7 +2541,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2736,11 +2735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="236438272"/>
-        <c:axId val="236439808"/>
+        <c:axId val="181867264"/>
+        <c:axId val="181868800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="236438272"/>
+        <c:axId val="181867264"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2749,7 +2748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236439808"/>
+        <c:crossAx val="181868800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2757,7 +2756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="236439808"/>
+        <c:axId val="181868800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2768,7 +2767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="236438272"/>
+        <c:crossAx val="181867264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3539,7 +3538,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3562,7 +3561,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="15">
-        <v>50000</v>
+        <v>48000</v>
       </c>
       <c r="C2" s="15">
         <v>65300</v>
@@ -3598,14 +3597,14 @@
       </c>
       <c r="B4" s="15">
         <f>D2*D3/100*D5*D4</f>
-        <v>21840</v>
+        <v>23520</v>
       </c>
       <c r="C4" s="15">
         <f>D2*D3*D7/100*D8</f>
-        <v>15456</v>
+        <v>12696</v>
       </c>
       <c r="D4">
-        <v>1.3</v>
+        <v>1.4</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>37</v>
@@ -3646,14 +3645,14 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <f>SUM(B2:B6)</f>
-        <v>97200</v>
+        <v>96880</v>
       </c>
       <c r="C7" s="15">
         <f>SUM(C2:C6)</f>
-        <v>97556</v>
+        <v>94796</v>
       </c>
       <c r="D7">
-        <v>0.28000000000000003</v>
+        <v>0.23</v>
       </c>
       <c r="E7" s="16" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
updated with latest D models
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -461,7 +461,7 @@
                   <c:v>45000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72400</c:v>
+                  <c:v>73900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -647,7 +647,7 @@
                 <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>20160</c:v>
+                  <c:v>17920</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7360</c:v>
@@ -805,11 +805,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="80177024"/>
-        <c:axId val="80178560"/>
+        <c:axId val="59132160"/>
+        <c:axId val="59158528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80177024"/>
+        <c:axId val="59132160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80178560"/>
+        <c:crossAx val="59158528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80178560"/>
+        <c:axId val="59158528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80177024"/>
+        <c:crossAx val="59132160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -987,7 +987,7 @@
                   <c:v>48000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>65300</c:v>
+                  <c:v>67900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1107,7 +1107,7 @@
                 <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23520</c:v>
+                  <c:v>21840</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>12696</c:v>
@@ -1268,11 +1268,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="80264192"/>
-        <c:axId val="80278272"/>
+        <c:axId val="59231616"/>
+        <c:axId val="59237504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80264192"/>
+        <c:axId val="59231616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80278272"/>
+        <c:crossAx val="59237504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1289,7 +1289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80278272"/>
+        <c:axId val="59237504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80264192"/>
+        <c:crossAx val="59231616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,11 +1546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="166757504"/>
-        <c:axId val="166759040"/>
+        <c:axId val="244286976"/>
+        <c:axId val="244288512"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="166757504"/>
+        <c:axId val="244286976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166759040"/>
+        <c:crossAx val="244288512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="166759040"/>
+        <c:axId val="244288512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1579,7 +1579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="166757504"/>
+        <c:crossAx val="244286976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1661,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181385472"/>
-        <c:axId val="181391360"/>
+        <c:axId val="76274304"/>
+        <c:axId val="76280192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181385472"/>
+        <c:axId val="76274304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181391360"/>
+        <c:crossAx val="76280192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181391360"/>
+        <c:axId val="76280192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1694,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181385472"/>
+        <c:crossAx val="76274304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1976,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181711616"/>
-        <c:axId val="181713152"/>
+        <c:axId val="76520832"/>
+        <c:axId val="76530816"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181711616"/>
+        <c:axId val="76520832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181713152"/>
+        <c:crossAx val="76530816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181713152"/>
+        <c:axId val="76530816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2019,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181711616"/>
+        <c:crossAx val="76520832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="181729152"/>
-        <c:axId val="181730688"/>
+        <c:axId val="76550528"/>
+        <c:axId val="76552064"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181729152"/>
+        <c:axId val="76550528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181730688"/>
+        <c:crossAx val="76552064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181730688"/>
+        <c:axId val="76552064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181729152"/>
+        <c:crossAx val="76550528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,11 +2438,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="181827456"/>
-        <c:axId val="181828992"/>
+        <c:axId val="75993472"/>
+        <c:axId val="75995008"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181827456"/>
+        <c:axId val="75993472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="181828992"/>
+        <c:crossAx val="75995008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2469,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181828992"/>
+        <c:axId val="75995008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181827456"/>
+        <c:crossAx val="75993472"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2735,11 +2735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="181867264"/>
-        <c:axId val="181868800"/>
+        <c:axId val="76016640"/>
+        <c:axId val="76169984"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="181867264"/>
+        <c:axId val="76016640"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2748,7 +2748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181868800"/>
+        <c:crossAx val="76169984"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2756,7 +2756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="181868800"/>
+        <c:axId val="76169984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="181867264"/>
+        <c:crossAx val="76016640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3381,8 +3381,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3408,7 +3408,7 @@
         <v>45000</v>
       </c>
       <c r="C2" s="6">
-        <v>72400</v>
+        <v>73900</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3447,7 +3447,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1.8</v>
+        <v>1.6</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -3459,7 +3459,7 @@
       </c>
       <c r="B5" s="6">
         <f>D2*D3/100*D5*D4</f>
-        <v>20160</v>
+        <v>17920</v>
       </c>
       <c r="C5" s="6">
         <f>D2*D3*D7/100*D8</f>
@@ -3507,11 +3507,11 @@
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B8" s="6">
         <f>SUM(B2:B7)</f>
-        <v>95760</v>
+        <v>93520</v>
       </c>
       <c r="C8" s="6">
         <f>SUM(C2:C7)</f>
-        <v>96560</v>
+        <v>98060</v>
       </c>
       <c r="D8">
         <v>23</v>
@@ -3538,7 +3538,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3564,7 +3564,7 @@
         <v>48000</v>
       </c>
       <c r="C2" s="15">
-        <v>65300</v>
+        <v>67900</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3597,14 +3597,14 @@
       </c>
       <c r="B4" s="15">
         <f>D2*D3/100*D5*D4</f>
-        <v>23520</v>
+        <v>21840</v>
       </c>
       <c r="C4" s="15">
         <f>D2*D3*D7/100*D8</f>
         <v>12696</v>
       </c>
       <c r="D4">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>37</v>
@@ -3645,11 +3645,11 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B7" s="15">
         <f>SUM(B2:B6)</f>
-        <v>96880</v>
+        <v>95200</v>
       </c>
       <c r="C7" s="15">
         <f>SUM(C2:C6)</f>
-        <v>94796</v>
+        <v>97396</v>
       </c>
       <c r="D7">
         <v>0.23</v>

</xml_diff>

<commit_message>
update S70D and make handout less technical. highlight supercharger network.
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten CHF" sheetId="2" r:id="rId1"/>
@@ -215,11 +215,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0&quot;min&quot;"/>
-    <numFmt numFmtId="165" formatCode="_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="166" formatCode="0\ &quot;Nm&quot;"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
     <numFmt numFmtId="168" formatCode="0\ &quot;L&quot;"/>
     <numFmt numFmtId="169" formatCode="0.0\ &quot;sec&quot;"/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* &quot;-&quot;\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="171" formatCode="_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -301,7 +301,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -320,7 +319,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -328,6 +326,8 @@
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -455,7 +455,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>45000</c:v>
@@ -513,7 +513,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1800</c:v>
@@ -575,7 +575,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2400</c:v>
@@ -644,7 +644,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>17920</c:v>
@@ -714,7 +714,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>16000</c:v>
@@ -783,7 +783,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$7:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * "-"??_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10400</c:v>
@@ -805,11 +805,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="59132160"/>
-        <c:axId val="59158528"/>
+        <c:axId val="56785152"/>
+        <c:axId val="56811520"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59132160"/>
+        <c:axId val="56785152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59158528"/>
+        <c:crossAx val="56811520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,18 +826,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59158528"/>
+        <c:axId val="56811520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_ [$Fr.-807]\ * #,##0.00_ ;_ [$Fr.-807]\ * \-#,##0.00_ ;_ [$Fr.-807]\ * &quot;-&quot;??_ ;_ @_ " sourceLinked="1"/>
+        <c:numFmt formatCode="_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * &quot;-&quot;_ ;_ @_ " sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59132160"/>
+        <c:crossAx val="56785152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -981,7 +981,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$2:$C$2</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>48000</c:v>
@@ -1039,7 +1039,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2160</c:v>
@@ -1104,7 +1104,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>21840</c:v>
@@ -1176,7 +1176,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>16000</c:v>
@@ -1246,7 +1246,7 @@
             <c:numRef>
               <c:f>'Kosten EUR'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_-* #\,##0.00\ [$€-407]_-;\-* #\,##0.00\ [$€-407]_-;_-* "-"??\ [$€-407]_-;_-@_-</c:formatCode>
+                <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>7200</c:v>
@@ -1268,11 +1268,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="59231616"/>
-        <c:axId val="59237504"/>
+        <c:axId val="56868224"/>
+        <c:axId val="56882304"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59231616"/>
+        <c:axId val="56868224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59237504"/>
+        <c:crossAx val="56882304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1289,18 +1289,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="59237504"/>
+        <c:axId val="56882304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-" sourceLinked="1"/>
+        <c:numFmt formatCode="_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* &quot;-&quot;\ [$€-407]_-;_-@_-" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59231616"/>
+        <c:crossAx val="56868224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,11 +1546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="244286976"/>
-        <c:axId val="244288512"/>
+        <c:axId val="246326784"/>
+        <c:axId val="246328320"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="244286976"/>
+        <c:axId val="246326784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244288512"/>
+        <c:crossAx val="246328320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="244288512"/>
+        <c:axId val="246328320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1579,7 +1579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="244286976"/>
+        <c:crossAx val="246326784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1661,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76274304"/>
-        <c:axId val="76280192"/>
+        <c:axId val="260885120"/>
+        <c:axId val="260895104"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76274304"/>
+        <c:axId val="260885120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76280192"/>
+        <c:crossAx val="260895104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76280192"/>
+        <c:axId val="260895104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1694,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76274304"/>
+        <c:crossAx val="260885120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1976,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76520832"/>
-        <c:axId val="76530816"/>
+        <c:axId val="261141632"/>
+        <c:axId val="261143168"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76520832"/>
+        <c:axId val="261141632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76530816"/>
+        <c:crossAx val="261143168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76530816"/>
+        <c:axId val="261143168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2019,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="76520832"/>
+        <c:crossAx val="261141632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="76550528"/>
-        <c:axId val="76552064"/>
+        <c:axId val="260898176"/>
+        <c:axId val="261150976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76550528"/>
+        <c:axId val="260898176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76552064"/>
+        <c:crossAx val="261150976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76552064"/>
+        <c:axId val="261150976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76550528"/>
+        <c:crossAx val="260898176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,11 +2438,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="75993472"/>
-        <c:axId val="75995008"/>
+        <c:axId val="260612480"/>
+        <c:axId val="260614016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="75993472"/>
+        <c:axId val="260612480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75995008"/>
+        <c:crossAx val="260614016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2469,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75995008"/>
+        <c:axId val="260614016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75993472"/>
+        <c:crossAx val="260612480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2735,11 +2735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="76016640"/>
-        <c:axId val="76169984"/>
+        <c:axId val="260709376"/>
+        <c:axId val="260727552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="76016640"/>
+        <c:axId val="260709376"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2748,7 +2748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76169984"/>
+        <c:crossAx val="260727552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2756,7 +2756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76169984"/>
+        <c:axId val="260727552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76016640"/>
+        <c:crossAx val="260709376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3381,8 +3381,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3404,10 +3404,10 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6">
+      <c r="B2" s="20">
         <v>45000</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="20">
         <v>73900</v>
       </c>
       <c r="D2">
@@ -3421,11 +3421,11 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="20">
         <f>0.04*B2</f>
         <v>1800</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="20">
         <v>0</v>
       </c>
       <c r="D3">
@@ -3439,11 +3439,11 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="20">
         <f>D2*300</f>
         <v>2400</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="20">
         <v>0</v>
       </c>
       <c r="D4">
@@ -3457,11 +3457,11 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="20">
         <f>D2*D3/100*D5*D4</f>
         <v>17920</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="20">
         <f>D2*D3*D7/100*D8</f>
         <v>7360</v>
       </c>
@@ -3476,11 +3476,11 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="20">
         <f>D2*2000</f>
         <v>16000</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="20">
         <f>D2*1500</f>
         <v>12000</v>
       </c>
@@ -3489,11 +3489,11 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="20">
         <f>D2*1300</f>
         <v>10400</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="20">
         <f>D2*600</f>
         <v>4800</v>
       </c>
@@ -3505,11 +3505,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="6">
+      <c r="B8" s="20">
         <f>SUM(B2:B7)</f>
         <v>93520</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="20">
         <f>SUM(C2:C7)</f>
         <v>98060</v>
       </c>
@@ -3537,8 +3537,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3549,7 +3549,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>39</v>
       </c>
       <c r="C1" t="s">
@@ -3560,10 +3560,10 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="19">
         <v>48000</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="19">
         <v>67900</v>
       </c>
       <c r="D2">
@@ -3577,11 +3577,11 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="19">
         <f>D2*270</f>
         <v>2160</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C3" s="19">
         <v>0</v>
       </c>
       <c r="D3">
@@ -3595,18 +3595,18 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="19">
         <f>D2*D3/100*D5*D4</f>
         <v>21840</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="19">
         <f>D2*D3*D7/100*D8</f>
         <v>12696</v>
       </c>
       <c r="D4">
         <v>1.3</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="14" t="s">
         <v>37</v>
       </c>
     </row>
@@ -3614,11 +3614,11 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="19">
         <f>D2*2000</f>
         <v>16000</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="19">
         <f>D2*1500</f>
         <v>12000</v>
       </c>
@@ -3633,28 +3633,28 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="19">
         <f>D2*900</f>
         <v>7200</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="19">
         <f>D2*600</f>
         <v>4800</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="15">
+      <c r="B7" s="19">
         <f>SUM(B2:B6)</f>
         <v>95200</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="19">
         <f>SUM(C2:C6)</f>
         <v>97396</v>
       </c>
       <c r="D7">
         <v>0.23</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="14" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3669,7 +3669,8 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3709,10 +3710,10 @@
       </c>
     </row>
     <row r="20" spans="2:4" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="13" t="s">
+      <c r="C20" s="12" t="s">
         <v>34</v>
       </c>
       <c r="D20" s="5">
@@ -3720,10 +3721,10 @@
       </c>
     </row>
     <row r="21" spans="2:4" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="12" t="s">
         <v>35</v>
       </c>
       <c r="D21" s="5">
@@ -3799,10 +3800,10 @@
       <c r="B6" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <v>550</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>450</v>
       </c>
     </row>
@@ -3818,11 +3819,11 @@
       <c r="B8" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="11">
         <f>C6*4.171</f>
         <v>2294.0500000000002</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <f>D6*9.73</f>
         <v>4378.5</v>
       </c>
@@ -3831,51 +3832,51 @@
       <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9" s="11">
         <f>C6*2.34</f>
         <v>1287</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="11"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <f>C6*1.521</f>
         <v>836.55</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="11"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <f>C6*1.143</f>
         <v>628.65</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="11"/>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <f>C6*0.867</f>
         <v>476.85</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="11"/>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <f>C6*0.691</f>
         <v>380.04999999999995</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -3900,301 +3901,301 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="7.25" style="7" customWidth="1"/>
-    <col min="5" max="5" width="10.75" style="7"/>
+    <col min="4" max="4" width="7.25" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10.75" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="8"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>700</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <f>A2/1.6</f>
         <v>437.5</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="8">
         <v>440</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>650</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <f t="shared" ref="B3:B16" si="0">A3/1.6</f>
         <v>406.25</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="9">
+      <c r="C3" s="18"/>
+      <c r="D3" s="8">
         <v>405</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>600</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="9">
+      <c r="C4" s="18"/>
+      <c r="D4" s="8">
         <v>375</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>550</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <f t="shared" si="0"/>
         <v>343.75</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="9">
+      <c r="C5" s="18"/>
+      <c r="D5" s="8">
         <v>345</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>500</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="9">
+      <c r="C6" s="18"/>
+      <c r="D6" s="8">
         <v>310</v>
       </c>
-      <c r="E6" s="11" t="s">
+      <c r="E6" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>450</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <f t="shared" si="0"/>
         <v>281.25</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="9">
+      <c r="C7" s="18"/>
+      <c r="D7" s="8">
         <v>280</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>400</v>
       </c>
-      <c r="B8" s="10">
+      <c r="B8" s="9">
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="9">
+      <c r="C8" s="18"/>
+      <c r="D8" s="8">
         <v>250</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>350</v>
       </c>
-      <c r="B9" s="10">
+      <c r="B9" s="9">
         <f t="shared" si="0"/>
         <v>218.75</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="9">
+      <c r="C9" s="18"/>
+      <c r="D9" s="8">
         <v>220</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>300</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="9">
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="9">
+      <c r="C10" s="18"/>
+      <c r="D10" s="8">
         <v>190</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>250</v>
       </c>
-      <c r="B11" s="10">
+      <c r="B11" s="9">
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="9">
+      <c r="C11" s="18"/>
+      <c r="D11" s="8">
         <v>160</v>
       </c>
-      <c r="E11" s="11" t="s">
+      <c r="E11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>200</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="9">
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="9">
+      <c r="C12" s="18"/>
+      <c r="D12" s="8">
         <v>125</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>150</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="9">
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="9">
+      <c r="C13" s="18"/>
+      <c r="D13" s="8">
         <v>100</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="9">
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="9">
+      <c r="C14" s="18"/>
+      <c r="D14" s="8">
         <v>65</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>50</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="9">
+      <c r="C15" s="18"/>
+      <c r="D15" s="8">
         <v>30</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="9">
+      <c r="C16" s="18"/>
+      <c r="D16" s="8">
         <v>0</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="8"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="9"/>
-      <c r="F18" s="8"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="8"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="8"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4653,7 +4654,7 @@
       <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="D2" s="16" t="s">
         <v>46</v>
       </c>
       <c r="E2" t="s">
@@ -4664,36 +4665,36 @@
       <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="15">
         <v>744.7</v>
       </c>
-      <c r="C3" s="17">
+      <c r="C3" s="15">
         <v>565</v>
       </c>
-      <c r="D3" s="17">
+      <c r="D3" s="15">
         <v>560</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="15">
         <v>485</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="15">
         <f>B6-B3</f>
         <v>900.5</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="15">
         <f>C6-C3</f>
         <v>1115</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="15">
         <f>D6-D3</f>
         <v>1110</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="15">
         <f>E6-E3</f>
         <v>1156</v>
       </c>
@@ -4702,30 +4703,30 @@
       <c r="A5" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="15">
         <v>150.1</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>0</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="15">
         <v>0</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="15">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="17">
+      <c r="B6" s="15">
         <v>1645.2</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="15">
         <v>1680</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="15">
         <v>1670</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="15">
         <v>1641</v>
       </c>
     </row>
@@ -4783,28 +4784,28 @@
       <c r="A3" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="17">
         <v>4.4000000000000004</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="17">
         <v>5.6</v>
       </c>
-      <c r="D3" s="19">
+      <c r="D3" s="17">
         <v>6.2</v>
       </c>
-      <c r="E3" s="19">
+      <c r="E3" s="17">
         <v>4.5</v>
       </c>
-      <c r="F3" s="19">
+      <c r="F3" s="17">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="17">
         <v>5.4</v>
       </c>
-      <c r="H3" s="19">
+      <c r="H3" s="17">
         <v>10.1</v>
       </c>
-      <c r="I3" s="19">
+      <c r="I3" s="17">
         <v>10.8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
base price for tesla adjusted. higher price for ICE with all wheel drive for fair comparison.
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -215,11 +215,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="0&quot;min&quot;"/>
-    <numFmt numFmtId="166" formatCode="0\ &quot;Nm&quot;"/>
-    <numFmt numFmtId="168" formatCode="0\ &quot;L&quot;"/>
-    <numFmt numFmtId="169" formatCode="0.0\ &quot;sec&quot;"/>
-    <numFmt numFmtId="170" formatCode="_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* &quot;-&quot;\ [$€-407]_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="0\ &quot;Nm&quot;"/>
+    <numFmt numFmtId="166" formatCode="0\ &quot;L&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.0\ &quot;sec&quot;"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* &quot;-&quot;\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -312,7 +312,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -320,14 +320,14 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -458,10 +458,10 @@
                 <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>45000</c:v>
+                  <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73900</c:v>
+                  <c:v>73100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,7 +516,7 @@
                 <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1800</c:v>
+                  <c:v>2200</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -575,7 +575,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #\,##0_ ;_ [$Fr.-807]\ * \-#\,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2400</c:v>
@@ -644,7 +644,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #\,##0_ ;_ [$Fr.-807]\ * \-#\,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>17920</c:v>
@@ -714,7 +714,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$6:$C$6</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #\,##0_ ;_ [$Fr.-807]\ * \-#\,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>16000</c:v>
@@ -783,7 +783,7 @@
             <c:numRef>
               <c:f>'Kosten CHF'!$B$7:$C$7</c:f>
               <c:numCache>
-                <c:formatCode>_ [$Fr.-807]\ * #,##0_ ;_ [$Fr.-807]\ * \-#,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
+                <c:formatCode>_ [$Fr.-807]\ * #\,##0_ ;_ [$Fr.-807]\ * \-#\,##0_ ;_ [$Fr.-807]\ * "-"_ ;_ @_ </c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>10400</c:v>
@@ -805,11 +805,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="56785152"/>
-        <c:axId val="56811520"/>
+        <c:axId val="80247040"/>
+        <c:axId val="80269312"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56785152"/>
+        <c:axId val="80247040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -818,7 +818,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56811520"/>
+        <c:crossAx val="80269312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -826,7 +826,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56811520"/>
+        <c:axId val="80269312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -837,7 +837,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56785152"/>
+        <c:crossAx val="80247040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -984,10 +984,10 @@
                 <c:formatCode>_-* #,##0\ [$€-407]_-;\-* #,##0\ [$€-407]_-;_-* "-"\ [$€-407]_-;_-@_-</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>48000</c:v>
+                  <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67900</c:v>
+                  <c:v>75800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1268,11 +1268,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="56868224"/>
-        <c:axId val="56882304"/>
+        <c:axId val="80338304"/>
+        <c:axId val="186975360"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="56868224"/>
+        <c:axId val="80338304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1281,7 +1281,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56882304"/>
+        <c:crossAx val="186975360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1289,7 +1289,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56882304"/>
+        <c:axId val="186975360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1300,7 +1300,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56868224"/>
+        <c:crossAx val="80338304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1546,11 +1546,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="246326784"/>
-        <c:axId val="246328320"/>
+        <c:axId val="187016704"/>
+        <c:axId val="187018240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="246326784"/>
+        <c:axId val="187016704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1559,7 +1559,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246328320"/>
+        <c:crossAx val="187018240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1567,7 +1567,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="246328320"/>
+        <c:axId val="187018240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1579,7 +1579,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="246326784"/>
+        <c:crossAx val="187016704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1661,11 +1661,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="260885120"/>
-        <c:axId val="260895104"/>
+        <c:axId val="203938432"/>
+        <c:axId val="209453440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260885120"/>
+        <c:axId val="203938432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1674,7 +1674,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260895104"/>
+        <c:crossAx val="209453440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1682,7 +1682,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260895104"/>
+        <c:axId val="209453440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1694,7 +1694,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260885120"/>
+        <c:crossAx val="203938432"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -1976,11 +1976,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="261141632"/>
-        <c:axId val="261143168"/>
+        <c:axId val="209499648"/>
+        <c:axId val="209501184"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="261141632"/>
+        <c:axId val="209499648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1989,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261143168"/>
+        <c:crossAx val="209501184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1997,7 +1997,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261143168"/>
+        <c:axId val="209501184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2019,7 +2019,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="261141632"/>
+        <c:crossAx val="209499648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2128,11 +2128,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="260898176"/>
-        <c:axId val="261150976"/>
+        <c:axId val="209508608"/>
+        <c:axId val="217649152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260898176"/>
+        <c:axId val="209508608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2141,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="261150976"/>
+        <c:crossAx val="217649152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="261150976"/>
+        <c:axId val="217649152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2160,7 +2160,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260898176"/>
+        <c:crossAx val="209508608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2438,11 +2438,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="260612480"/>
-        <c:axId val="260614016"/>
+        <c:axId val="217286912"/>
+        <c:axId val="217300992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260612480"/>
+        <c:axId val="217286912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2461,7 +2461,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="260614016"/>
+        <c:crossAx val="217300992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2469,7 +2469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260614016"/>
+        <c:axId val="217300992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2480,7 +2480,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260612480"/>
+        <c:crossAx val="217286912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2735,11 +2735,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="260709376"/>
-        <c:axId val="260727552"/>
+        <c:axId val="217334912"/>
+        <c:axId val="217336448"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="260709376"/>
+        <c:axId val="217334912"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2748,7 +2748,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260727552"/>
+        <c:crossAx val="217336448"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2756,7 +2756,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="260727552"/>
+        <c:axId val="217336448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2767,7 +2767,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="260709376"/>
+        <c:crossAx val="217334912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3382,7 +3382,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3404,11 +3404,11 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="20">
-        <v>45000</v>
-      </c>
-      <c r="C2" s="20">
-        <v>73900</v>
+      <c r="B2" s="19">
+        <v>55000</v>
+      </c>
+      <c r="C2" s="19">
+        <v>73100</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3421,11 +3421,11 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <f>0.04*B2</f>
-        <v>1800</v>
-      </c>
-      <c r="C3" s="20">
+        <v>2200</v>
+      </c>
+      <c r="C3" s="19">
         <v>0</v>
       </c>
       <c r="D3">
@@ -3439,11 +3439,11 @@
       <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <f>D2*300</f>
         <v>2400</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="19">
         <v>0</v>
       </c>
       <c r="D4">
@@ -3457,11 +3457,11 @@
       <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <f>D2*D3/100*D5*D4</f>
         <v>17920</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="19">
         <f>D2*D3*D7/100*D8</f>
         <v>7360</v>
       </c>
@@ -3476,11 +3476,11 @@
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="19">
         <f>D2*2000</f>
         <v>16000</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="19">
         <f>D2*1500</f>
         <v>12000</v>
       </c>
@@ -3489,11 +3489,11 @@
       <c r="A7" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="19">
         <f>D2*1300</f>
         <v>10400</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="19">
         <f>D2*600</f>
         <v>4800</v>
       </c>
@@ -3505,13 +3505,13 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="20">
+      <c r="B8" s="19">
         <f>SUM(B2:B7)</f>
-        <v>93520</v>
-      </c>
-      <c r="C8" s="20">
+        <v>103920</v>
+      </c>
+      <c r="C8" s="19">
         <f>SUM(C2:C7)</f>
-        <v>98060</v>
+        <v>97260</v>
       </c>
       <c r="D8">
         <v>23</v>
@@ -3538,7 +3538,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3560,11 +3560,11 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="19">
-        <v>48000</v>
-      </c>
-      <c r="C2" s="19">
-        <v>67900</v>
+      <c r="B2" s="18">
+        <v>55000</v>
+      </c>
+      <c r="C2" s="18">
+        <v>75800</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3577,11 +3577,11 @@
       <c r="A3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <f>D2*270</f>
         <v>2160</v>
       </c>
-      <c r="C3" s="19">
+      <c r="C3" s="18">
         <v>0</v>
       </c>
       <c r="D3">
@@ -3595,11 +3595,11 @@
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <f>D2*D3/100*D5*D4</f>
         <v>21840</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="18">
         <f>D2*D3*D7/100*D8</f>
         <v>12696</v>
       </c>
@@ -3614,11 +3614,11 @@
       <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <f>D2*2000</f>
         <v>16000</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <f>D2*1500</f>
         <v>12000</v>
       </c>
@@ -3633,23 +3633,23 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="18">
         <f>D2*900</f>
         <v>7200</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="18">
         <f>D2*600</f>
         <v>4800</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="19">
+      <c r="B7" s="18">
         <f>SUM(B2:B6)</f>
-        <v>95200</v>
-      </c>
-      <c r="C7" s="19">
+        <v>102200</v>
+      </c>
+      <c r="C7" s="18">
         <f>SUM(C2:C6)</f>
-        <v>97396</v>
+        <v>105296</v>
       </c>
       <c r="D7">
         <v>0.23</v>
@@ -3920,7 +3920,7 @@
         <f>A2/1.6</f>
         <v>437.5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>23</v>
       </c>
       <c r="D2" s="8">
@@ -3939,7 +3939,7 @@
         <f t="shared" ref="B3:B16" si="0">A3/1.6</f>
         <v>406.25</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="8">
         <v>405</v>
       </c>
@@ -3956,7 +3956,7 @@
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="8">
         <v>375</v>
       </c>
@@ -3973,7 +3973,7 @@
         <f t="shared" si="0"/>
         <v>343.75</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="8">
         <v>345</v>
       </c>
@@ -3990,7 +3990,7 @@
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="8">
         <v>310</v>
       </c>
@@ -4007,7 +4007,7 @@
         <f t="shared" si="0"/>
         <v>281.25</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>280</v>
       </c>
@@ -4024,7 +4024,7 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8">
         <v>250</v>
       </c>
@@ -4041,7 +4041,7 @@
         <f t="shared" si="0"/>
         <v>218.75</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8">
         <v>220</v>
       </c>
@@ -4058,7 +4058,7 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8">
         <v>190</v>
       </c>
@@ -4075,7 +4075,7 @@
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8">
         <v>160</v>
       </c>
@@ -4092,7 +4092,7 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="8">
         <v>125</v>
       </c>
@@ -4109,7 +4109,7 @@
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="8">
         <v>100</v>
       </c>
@@ -4126,7 +4126,7 @@
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8">
         <v>65</v>
       </c>
@@ -4143,7 +4143,7 @@
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8">
         <v>30</v>
       </c>
@@ -4160,7 +4160,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add forum essentials qr-tag. add chademo plug
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>|</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -207,6 +207,13 @@
   <si>
     <t>überall 
 (3Phasen, 400V)</t>
+  </si>
+  <si>
+    <t>öffentlich
+(CHAdeMO)</t>
+  </si>
+  <si>
+    <t>50kW</t>
   </si>
 </sst>
 </file>
@@ -315,14 +322,14 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -801,11 +808,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="80574720"/>
-        <c:axId val="80596992"/>
+        <c:axId val="52271360"/>
+        <c:axId val="52285440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80574720"/>
+        <c:axId val="52271360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -814,7 +821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80596992"/>
+        <c:crossAx val="52285440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -822,7 +829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80596992"/>
+        <c:axId val="52285440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -833,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80574720"/>
+        <c:crossAx val="52271360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1264,11 +1271,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="80665984"/>
-        <c:axId val="242881664"/>
+        <c:axId val="52358528"/>
+        <c:axId val="241771648"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80665984"/>
+        <c:axId val="52358528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1277,7 +1284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242881664"/>
+        <c:crossAx val="241771648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1285,7 +1292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242881664"/>
+        <c:axId val="241771648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80665984"/>
+        <c:crossAx val="52358528"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1463,8 +1470,8 @@
               <c:idx val="3"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0"/>
-                  <c:y val="1.3088066028813428E-2"/>
+                  <c:x val="8.4626929467710932E-17"/>
+                  <c:y val="7.5596328837500759E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1478,8 +1485,23 @@
               <c:idx val="4"/>
               <c:layout>
                 <c:manualLayout>
+                  <c:x val="-2.3082155645441659E-3"/>
+                  <c:y val="-6.1561861247261072E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="5"/>
+              <c:layout>
+                <c:manualLayout>
                   <c:x val="0"/>
-                  <c:y val="1.3193399591276106E-2"/>
+                  <c:y val="8.292698746714209E-3"/>
                 </c:manualLayout>
               </c:layout>
               <c:showLegendKey val="0"/>
@@ -1499,9 +1521,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'Ladedauer 100km'!$B$20:$C$24</c:f>
+              <c:f>'Ladedauer 100km'!$B$20:$C$25</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>2.3kW</c:v>
@@ -1516,6 +1538,9 @@
                     <c:v>22kW</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>50kW</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>120kW</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1536,6 +1561,10 @@
                     <c:v>öffentlich / zuhause (Typ2)</c:v>
                   </c:pt>
                   <c:pt idx="4">
+                    <c:v>öffentlich
+(CHAdeMO)</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
                     <c:v>Tesla Supercharger</c:v>
                   </c:pt>
                 </c:lvl>
@@ -1544,10 +1573,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Ladedauer 100km'!$D$20:$D$24</c:f>
+              <c:f>'Ladedauer 100km'!$D$20:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0"min"</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>600</c:v>
                 </c:pt>
@@ -1561,6 +1590,9 @@
                   <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
@@ -1576,11 +1608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="242923008"/>
-        <c:axId val="242924544"/>
+        <c:axId val="241812992"/>
+        <c:axId val="241814528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="242923008"/>
+        <c:axId val="241812992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1589,7 +1621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242924544"/>
+        <c:crossAx val="241814528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1597,7 +1629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="242924544"/>
+        <c:axId val="241814528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1609,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="242923008"/>
+        <c:crossAx val="241812992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1696,11 +1728,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="257481344"/>
-        <c:axId val="257687936"/>
+        <c:axId val="256392192"/>
+        <c:axId val="256398080"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257481344"/>
+        <c:axId val="256392192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257687936"/>
+        <c:crossAx val="256398080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1717,7 +1749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257687936"/>
+        <c:axId val="256398080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1729,7 +1761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257481344"/>
+        <c:crossAx val="256392192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -2011,11 +2043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="257738240"/>
-        <c:axId val="257739776"/>
+        <c:axId val="256649088"/>
+        <c:axId val="256650624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257738240"/>
+        <c:axId val="256649088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2024,7 +2056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257739776"/>
+        <c:crossAx val="256650624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2032,7 +2064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257739776"/>
+        <c:axId val="256650624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2054,7 +2086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257738240"/>
+        <c:crossAx val="256649088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2163,11 +2195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="257751296"/>
-        <c:axId val="258027520"/>
+        <c:axId val="256660608"/>
+        <c:axId val="256662144"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257751296"/>
+        <c:axId val="256660608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2176,7 +2208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="258027520"/>
+        <c:crossAx val="256662144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2184,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="258027520"/>
+        <c:axId val="256662144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2195,7 +2227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257751296"/>
+        <c:crossAx val="256660608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2473,11 +2505,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="257274240"/>
-        <c:axId val="257275776"/>
+        <c:axId val="256115840"/>
+        <c:axId val="256117376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257274240"/>
+        <c:axId val="256115840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2496,7 +2528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="257275776"/>
+        <c:crossAx val="256117376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2504,7 +2536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257275776"/>
+        <c:axId val="256117376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2515,7 +2547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257274240"/>
+        <c:crossAx val="256115840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2576,7 +2608,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2771,11 +2802,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="257301504"/>
-        <c:axId val="257315584"/>
+        <c:axId val="256151552"/>
+        <c:axId val="256153088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="257301504"/>
+        <c:axId val="256151552"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2784,7 +2815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257315584"/>
+        <c:crossAx val="256153088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2792,7 +2823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="257315584"/>
+        <c:axId val="256153088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2803,7 +2834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="257301504"/>
+        <c:crossAx val="256151552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -2973,16 +3004,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>54429</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>149678</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>114510</xdr:rowOff>
+      <xdr:rowOff>114511</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>54428</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>21981</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>140132</xdr:rowOff>
+      <xdr:rowOff>40271</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3006,8 +3037,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5307833" y="4378779"/>
-          <a:ext cx="857249" cy="670391"/>
+          <a:off x="5117332" y="4510665"/>
+          <a:ext cx="729553" cy="570529"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3028,16 +3059,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>176981</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>118363</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>88551</xdr:rowOff>
+      <xdr:rowOff>103205</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>72837</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>121208</xdr:rowOff>
+      <xdr:rowOff>37394</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3054,8 +3085,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6287635" y="4352820"/>
-          <a:ext cx="753106" cy="677426"/>
+          <a:off x="5943267" y="4499359"/>
+          <a:ext cx="643638" cy="578958"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3069,13 +3100,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>212271</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>38729</xdr:rowOff>
+      <xdr:rowOff>24076</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>168729</xdr:colOff>
+      <xdr:colOff>131884</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>59605</xdr:rowOff>
+      <xdr:rowOff>9747</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3099,8 +3130,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="4608425" y="4625383"/>
-          <a:ext cx="527958" cy="504453"/>
+          <a:off x="4608425" y="4742614"/>
+          <a:ext cx="491113" cy="469248"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3122,15 +3153,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>244929</xdr:colOff>
+      <xdr:colOff>244930</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>133503</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>119744</xdr:colOff>
+      <xdr:colOff>88598</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>95964</xdr:rowOff>
+      <xdr:rowOff>76086</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3147,8 +3178,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4641083" y="4397772"/>
-          <a:ext cx="446315" cy="284846"/>
+          <a:off x="4641084" y="4529657"/>
+          <a:ext cx="415168" cy="264967"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3159,16 +3190,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>195942</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>153866</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>42081</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>36637</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>2005</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>130057</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>119417</xdr:rowOff>
+      <xdr:rowOff>51289</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3179,13 +3210,50 @@
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
-        <a:srcRect l="14836" t="17630"/>
+        <a:srcRect l="14835" t="17630" r="12672"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7163846" y="4418135"/>
-          <a:ext cx="949063" cy="610320"/>
+          <a:off x="6724235" y="4593983"/>
+          <a:ext cx="659476" cy="498229"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>175846</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>131886</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>30119</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>124559</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:srcRect l="32580" r="4644"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="4528040"/>
+          <a:ext cx="711523" cy="637442"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3986,10 +4054,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A17:AD40"/>
+  <dimension ref="A17:AG40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="AB24" sqref="AB24"/>
+      <selection activeCell="AA20" sqref="AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4002,19 +4070,19 @@
     <col min="29" max="16384" width="4.125" style="1"/>
   </cols>
   <sheetData>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:33" x14ac:dyDescent="0.2">
       <c r="D17" s="4">
         <f>75/4*60</f>
         <v>1125</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:33" x14ac:dyDescent="0.2">
       <c r="D19" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="2:30" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B20" s="19" t="s">
+    <row r="20" spans="2:33" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B20" s="18" t="s">
         <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -4024,8 +4092,8 @@
         <v>600</v>
       </c>
     </row>
-    <row r="21" spans="2:30" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B21" s="19" t="s">
+    <row r="21" spans="2:33" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B21" s="18" t="s">
         <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
@@ -4035,8 +4103,8 @@
         <v>380</v>
       </c>
     </row>
-    <row r="22" spans="2:30" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="B22" s="19" t="s">
+    <row r="22" spans="2:33" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B22" s="18" t="s">
         <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -4046,7 +4114,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>8</v>
       </c>
@@ -4057,253 +4125,265 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="B24" s="4" t="s">
+    <row r="24" spans="2:33" ht="23.25" x14ac:dyDescent="0.2">
+      <c r="B24" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D25" s="5">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:33" x14ac:dyDescent="0.2">
       <c r="AD26"/>
-    </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AG26"/>
+    </row>
+    <row r="28" spans="2:33" x14ac:dyDescent="0.2">
       <c r="AC28"/>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="F30" s="20"/>
-      <c r="G30" s="20"/>
-      <c r="H30" s="20"/>
-      <c r="I30" s="20"/>
-      <c r="J30" s="20"/>
-      <c r="K30" s="20"/>
-      <c r="L30" s="20"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="20"/>
-      <c r="O30" s="20"/>
-      <c r="P30" s="20"/>
-      <c r="Q30" s="20"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="20"/>
-      <c r="T30" s="20"/>
-      <c r="U30" s="20"/>
-      <c r="V30" s="20"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="20"/>
-    </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="F31" s="20"/>
-      <c r="G31" s="20"/>
-      <c r="H31" s="20"/>
-      <c r="I31" s="20"/>
-      <c r="J31" s="20"/>
-      <c r="K31" s="20"/>
-      <c r="L31" s="20"/>
-      <c r="M31" s="20"/>
-      <c r="N31" s="20"/>
-      <c r="O31" s="20"/>
-      <c r="P31" s="20"/>
-      <c r="Q31" s="20"/>
-      <c r="R31" s="20"/>
-      <c r="S31" s="20"/>
-      <c r="T31" s="20"/>
-      <c r="U31" s="20"/>
-      <c r="V31" s="20"/>
-      <c r="W31" s="20"/>
-      <c r="X31" s="20"/>
-    </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.2">
-      <c r="F32" s="20"/>
-      <c r="G32" s="20"/>
-      <c r="H32" s="20"/>
-      <c r="I32" s="20"/>
-      <c r="J32" s="20"/>
-      <c r="K32" s="20"/>
-      <c r="L32" s="20"/>
-      <c r="M32" s="20"/>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
-      <c r="S32" s="20"/>
-      <c r="T32" s="20"/>
-      <c r="U32" s="20"/>
-      <c r="V32" s="20"/>
-      <c r="W32" s="20"/>
-      <c r="X32" s="20"/>
+    <row r="30" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="19"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
+      <c r="S30" s="19"/>
+      <c r="T30" s="19"/>
+      <c r="U30" s="19"/>
+      <c r="V30" s="19"/>
+      <c r="W30" s="19"/>
+      <c r="X30" s="19"/>
+    </row>
+    <row r="31" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="19"/>
+      <c r="K31" s="19"/>
+      <c r="L31" s="19"/>
+      <c r="M31" s="19"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
+      <c r="S31" s="19"/>
+      <c r="T31" s="19"/>
+      <c r="U31" s="19"/>
+      <c r="V31" s="19"/>
+      <c r="W31" s="19"/>
+      <c r="X31" s="19"/>
+    </row>
+    <row r="32" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="H32" s="19"/>
+      <c r="I32" s="19"/>
+      <c r="J32" s="19"/>
+      <c r="K32" s="19"/>
+      <c r="L32" s="19"/>
+      <c r="M32" s="19"/>
+      <c r="N32" s="19"/>
+      <c r="O32" s="19"/>
+      <c r="P32" s="19"/>
+      <c r="Q32" s="19"/>
+      <c r="R32" s="19"/>
+      <c r="S32" s="19"/>
+      <c r="T32" s="19"/>
+      <c r="U32" s="19"/>
+      <c r="V32" s="19"/>
+      <c r="W32" s="19"/>
+      <c r="X32" s="19"/>
     </row>
     <row r="33" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F33" s="20"/>
-      <c r="G33" s="20"/>
-      <c r="H33" s="20"/>
-      <c r="I33" s="20"/>
-      <c r="J33" s="20"/>
-      <c r="K33" s="20"/>
-      <c r="L33" s="20"/>
-      <c r="M33" s="20"/>
-      <c r="N33" s="20"/>
-      <c r="O33" s="20"/>
-      <c r="P33" s="20"/>
-      <c r="Q33" s="20"/>
-      <c r="R33" s="20"/>
-      <c r="S33" s="20"/>
-      <c r="T33" s="20"/>
-      <c r="U33" s="20"/>
-      <c r="V33" s="20"/>
-      <c r="W33" s="20"/>
-      <c r="X33" s="20"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="H33" s="19"/>
+      <c r="I33" s="19"/>
+      <c r="J33" s="19"/>
+      <c r="K33" s="19"/>
+      <c r="L33" s="19"/>
+      <c r="M33" s="19"/>
+      <c r="N33" s="19"/>
+      <c r="O33" s="19"/>
+      <c r="P33" s="19"/>
+      <c r="Q33" s="19"/>
+      <c r="R33" s="19"/>
+      <c r="S33" s="19"/>
+      <c r="T33" s="19"/>
+      <c r="U33" s="19"/>
+      <c r="V33" s="19"/>
+      <c r="W33" s="19"/>
+      <c r="X33" s="19"/>
     </row>
     <row r="34" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F34" s="20"/>
-      <c r="G34" s="20"/>
-      <c r="H34" s="20"/>
-      <c r="I34" s="20"/>
-      <c r="J34" s="20"/>
-      <c r="K34" s="20"/>
-      <c r="L34" s="20"/>
-      <c r="M34" s="20"/>
-      <c r="N34" s="20"/>
-      <c r="O34" s="20"/>
-      <c r="P34" s="20"/>
-      <c r="Q34" s="20"/>
-      <c r="R34" s="20"/>
-      <c r="S34" s="20"/>
-      <c r="T34" s="20"/>
-      <c r="U34" s="20"/>
-      <c r="V34" s="20"/>
-      <c r="W34" s="20"/>
-      <c r="X34" s="20"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
     </row>
     <row r="35" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="20"/>
-      <c r="I35" s="20"/>
-      <c r="J35" s="20"/>
-      <c r="K35" s="20"/>
-      <c r="L35" s="20"/>
-      <c r="M35" s="20"/>
-      <c r="N35" s="20"/>
-      <c r="O35" s="20"/>
-      <c r="P35" s="20"/>
-      <c r="Q35" s="20"/>
-      <c r="R35" s="20"/>
-      <c r="S35" s="20"/>
-      <c r="T35" s="20"/>
-      <c r="U35" s="20"/>
-      <c r="V35" s="20"/>
-      <c r="W35" s="20"/>
-      <c r="X35" s="20"/>
+      <c r="F35" s="19"/>
+      <c r="G35" s="19"/>
+      <c r="H35" s="19"/>
+      <c r="I35" s="19"/>
+      <c r="J35" s="19"/>
+      <c r="K35" s="19"/>
+      <c r="L35" s="19"/>
+      <c r="M35" s="19"/>
+      <c r="N35" s="19"/>
+      <c r="O35" s="19"/>
+      <c r="P35" s="19"/>
+      <c r="Q35" s="19"/>
+      <c r="R35" s="19"/>
+      <c r="S35" s="19"/>
+      <c r="T35" s="19"/>
+      <c r="U35" s="19"/>
+      <c r="V35" s="19"/>
+      <c r="W35" s="19"/>
+      <c r="X35" s="19"/>
     </row>
     <row r="36" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-      <c r="L36" s="20"/>
-      <c r="M36" s="20"/>
-      <c r="N36" s="20"/>
-      <c r="O36" s="20"/>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="20"/>
-      <c r="R36" s="20"/>
-      <c r="S36" s="20"/>
-      <c r="T36" s="20"/>
-      <c r="U36" s="20"/>
-      <c r="V36" s="20"/>
-      <c r="W36" s="20"/>
-      <c r="X36" s="20"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+      <c r="N36" s="19"/>
+      <c r="O36" s="19"/>
+      <c r="P36" s="19"/>
+      <c r="Q36" s="19"/>
+      <c r="R36" s="19"/>
+      <c r="S36" s="19"/>
+      <c r="T36" s="19"/>
+      <c r="U36" s="19"/>
+      <c r="V36" s="19"/>
+      <c r="W36" s="19"/>
+      <c r="X36" s="19"/>
     </row>
     <row r="37" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="20"/>
-      <c r="I37" s="20"/>
-      <c r="J37" s="20"/>
-      <c r="K37" s="20"/>
-      <c r="L37" s="20"/>
-      <c r="M37" s="20"/>
-      <c r="N37" s="20"/>
-      <c r="O37" s="20"/>
-      <c r="P37" s="20"/>
-      <c r="Q37" s="20"/>
-      <c r="R37" s="20"/>
-      <c r="S37" s="20"/>
-      <c r="T37" s="20"/>
-      <c r="U37" s="20"/>
-      <c r="V37" s="20"/>
-      <c r="W37" s="20"/>
-      <c r="X37" s="20"/>
+      <c r="F37" s="19"/>
+      <c r="G37" s="19"/>
+      <c r="H37" s="19"/>
+      <c r="I37" s="19"/>
+      <c r="J37" s="19"/>
+      <c r="K37" s="19"/>
+      <c r="L37" s="19"/>
+      <c r="M37" s="19"/>
+      <c r="N37" s="19"/>
+      <c r="O37" s="19"/>
+      <c r="P37" s="19"/>
+      <c r="Q37" s="19"/>
+      <c r="R37" s="19"/>
+      <c r="S37" s="19"/>
+      <c r="T37" s="19"/>
+      <c r="U37" s="19"/>
+      <c r="V37" s="19"/>
+      <c r="W37" s="19"/>
+      <c r="X37" s="19"/>
     </row>
     <row r="38" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F38" s="20"/>
-      <c r="G38" s="20"/>
-      <c r="H38" s="20"/>
-      <c r="I38" s="20"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
-      <c r="P38" s="20"/>
-      <c r="Q38" s="20"/>
-      <c r="R38" s="20"/>
-      <c r="S38" s="20"/>
-      <c r="T38" s="20"/>
-      <c r="U38" s="20"/>
-      <c r="V38" s="20"/>
-      <c r="W38" s="20"/>
-      <c r="X38" s="20"/>
+      <c r="F38" s="19"/>
+      <c r="G38" s="19"/>
+      <c r="H38" s="19"/>
+      <c r="I38" s="19"/>
+      <c r="J38" s="19"/>
+      <c r="K38" s="19"/>
+      <c r="L38" s="19"/>
+      <c r="M38" s="19"/>
+      <c r="N38" s="19"/>
+      <c r="O38" s="19"/>
+      <c r="P38" s="19"/>
+      <c r="Q38" s="19"/>
+      <c r="R38" s="19"/>
+      <c r="S38" s="19"/>
+      <c r="T38" s="19"/>
+      <c r="U38" s="19"/>
+      <c r="V38" s="19"/>
+      <c r="W38" s="19"/>
+      <c r="X38" s="19"/>
     </row>
     <row r="39" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
-      <c r="P39" s="20"/>
-      <c r="Q39" s="20"/>
-      <c r="R39" s="20"/>
-      <c r="S39" s="20"/>
-      <c r="T39" s="20"/>
-      <c r="U39" s="20"/>
-      <c r="V39" s="20"/>
-      <c r="W39" s="20"/>
-      <c r="X39" s="20"/>
+      <c r="F39" s="19"/>
+      <c r="G39" s="19"/>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
+      <c r="J39" s="19"/>
+      <c r="K39" s="19"/>
+      <c r="L39" s="19"/>
+      <c r="M39" s="19"/>
+      <c r="N39" s="19"/>
+      <c r="O39" s="19"/>
+      <c r="P39" s="19"/>
+      <c r="Q39" s="19"/>
+      <c r="R39" s="19"/>
+      <c r="S39" s="19"/>
+      <c r="T39" s="19"/>
+      <c r="U39" s="19"/>
+      <c r="V39" s="19"/>
+      <c r="W39" s="19"/>
+      <c r="X39" s="19"/>
     </row>
     <row r="40" spans="6:24" x14ac:dyDescent="0.2">
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
-      <c r="P40" s="20"/>
-      <c r="Q40" s="20"/>
-      <c r="R40" s="20"/>
-      <c r="S40" s="20"/>
-      <c r="T40" s="20"/>
-      <c r="U40" s="20"/>
-      <c r="V40" s="20"/>
-      <c r="W40" s="20"/>
-      <c r="X40" s="20"/>
+      <c r="F40" s="19"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="19"/>
+      <c r="I40" s="19"/>
+      <c r="J40" s="19"/>
+      <c r="K40" s="19"/>
+      <c r="L40" s="19"/>
+      <c r="M40" s="19"/>
+      <c r="N40" s="19"/>
+      <c r="O40" s="19"/>
+      <c r="P40" s="19"/>
+      <c r="Q40" s="19"/>
+      <c r="R40" s="19"/>
+      <c r="S40" s="19"/>
+      <c r="T40" s="19"/>
+      <c r="U40" s="19"/>
+      <c r="V40" s="19"/>
+      <c r="W40" s="19"/>
+      <c r="X40" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -4461,7 +4541,7 @@
         <f>A2/1.6</f>
         <v>437.5</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="20" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="8">
@@ -4480,7 +4560,7 @@
         <f t="shared" ref="B3:B16" si="0">A3/1.6</f>
         <v>406.25</v>
       </c>
-      <c r="C3" s="18"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="8">
         <v>405</v>
       </c>
@@ -4497,7 +4577,7 @@
         <f t="shared" si="0"/>
         <v>375</v>
       </c>
-      <c r="C4" s="18"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="8">
         <v>375</v>
       </c>
@@ -4514,7 +4594,7 @@
         <f t="shared" si="0"/>
         <v>343.75</v>
       </c>
-      <c r="C5" s="18"/>
+      <c r="C5" s="20"/>
       <c r="D5" s="8">
         <v>345</v>
       </c>
@@ -4531,7 +4611,7 @@
         <f t="shared" si="0"/>
         <v>312.5</v>
       </c>
-      <c r="C6" s="18"/>
+      <c r="C6" s="20"/>
       <c r="D6" s="8">
         <v>310</v>
       </c>
@@ -4548,7 +4628,7 @@
         <f t="shared" si="0"/>
         <v>281.25</v>
       </c>
-      <c r="C7" s="18"/>
+      <c r="C7" s="20"/>
       <c r="D7" s="8">
         <v>280</v>
       </c>
@@ -4565,7 +4645,7 @@
         <f t="shared" si="0"/>
         <v>250</v>
       </c>
-      <c r="C8" s="18"/>
+      <c r="C8" s="20"/>
       <c r="D8" s="8">
         <v>250</v>
       </c>
@@ -4582,7 +4662,7 @@
         <f t="shared" si="0"/>
         <v>218.75</v>
       </c>
-      <c r="C9" s="18"/>
+      <c r="C9" s="20"/>
       <c r="D9" s="8">
         <v>220</v>
       </c>
@@ -4599,7 +4679,7 @@
         <f t="shared" si="0"/>
         <v>187.5</v>
       </c>
-      <c r="C10" s="18"/>
+      <c r="C10" s="20"/>
       <c r="D10" s="8">
         <v>190</v>
       </c>
@@ -4616,7 +4696,7 @@
         <f t="shared" si="0"/>
         <v>156.25</v>
       </c>
-      <c r="C11" s="18"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8">
         <v>160</v>
       </c>
@@ -4633,7 +4713,7 @@
         <f t="shared" si="0"/>
         <v>125</v>
       </c>
-      <c r="C12" s="18"/>
+      <c r="C12" s="20"/>
       <c r="D12" s="8">
         <v>125</v>
       </c>
@@ -4650,7 +4730,7 @@
         <f t="shared" si="0"/>
         <v>93.75</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="20"/>
       <c r="D13" s="8">
         <v>100</v>
       </c>
@@ -4667,7 +4747,7 @@
         <f t="shared" si="0"/>
         <v>62.5</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="20"/>
       <c r="D14" s="8">
         <v>65</v>
       </c>
@@ -4684,7 +4764,7 @@
         <f t="shared" si="0"/>
         <v>31.25</v>
       </c>
-      <c r="C15" s="18"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="8">
         <v>30</v>
       </c>
@@ -4701,7 +4781,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="C16" s="18"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="8">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
updated with information about model x
</commit_message>
<xml_diff>
--- a/tesla_charts.xlsx
+++ b/tesla_charts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="-15" windowWidth="25440" windowHeight="13320" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Kosten CHF" sheetId="2" r:id="rId1"/>
@@ -464,7 +464,7 @@
                   <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73100</c:v>
+                  <c:v>74500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -808,11 +808,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="52271360"/>
-        <c:axId val="52285440"/>
+        <c:axId val="275629184"/>
+        <c:axId val="275630720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52271360"/>
+        <c:axId val="275629184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -821,7 +821,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52285440"/>
+        <c:crossAx val="275630720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -829,7 +829,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52285440"/>
+        <c:axId val="275630720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -840,7 +840,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52271360"/>
+        <c:crossAx val="275629184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -990,7 +990,7 @@
                   <c:v>55000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>75800</c:v>
+                  <c:v>78000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,11 +1271,11 @@
         </c:dLbls>
         <c:gapWidth val="27"/>
         <c:overlap val="100"/>
-        <c:axId val="52358528"/>
-        <c:axId val="241771648"/>
+        <c:axId val="303659264"/>
+        <c:axId val="303665152"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="52358528"/>
+        <c:axId val="303659264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1284,7 +1284,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241771648"/>
+        <c:crossAx val="303665152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1292,7 +1292,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241771648"/>
+        <c:axId val="303665152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1303,7 +1303,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52358528"/>
+        <c:crossAx val="303659264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1608,11 +1608,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="40"/>
-        <c:axId val="241812992"/>
-        <c:axId val="241814528"/>
+        <c:axId val="304882048"/>
+        <c:axId val="304883584"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="241812992"/>
+        <c:axId val="304882048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1621,7 +1621,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241814528"/>
+        <c:crossAx val="304883584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1629,7 +1629,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="241814528"/>
+        <c:axId val="304883584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -1641,7 +1641,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="241812992"/>
+        <c:crossAx val="304882048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="50"/>
@@ -1728,11 +1728,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256392192"/>
-        <c:axId val="256398080"/>
+        <c:axId val="304978176"/>
+        <c:axId val="304979968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256392192"/>
+        <c:axId val="304978176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1741,7 +1741,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256398080"/>
+        <c:crossAx val="304979968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1749,7 +1749,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256398080"/>
+        <c:axId val="304979968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -1761,7 +1761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256392192"/>
+        <c:crossAx val="304978176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="500"/>
@@ -2043,11 +2043,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256649088"/>
-        <c:axId val="256650624"/>
+        <c:axId val="305486848"/>
+        <c:axId val="305488640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256649088"/>
+        <c:axId val="305486848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2056,7 +2056,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256650624"/>
+        <c:crossAx val="305488640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2064,7 +2064,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256650624"/>
+        <c:axId val="305488640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="5000"/>
@@ -2086,7 +2086,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256649088"/>
+        <c:crossAx val="305486848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2195,11 +2195,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="256660608"/>
-        <c:axId val="256662144"/>
+        <c:axId val="305512832"/>
+        <c:axId val="305514368"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256660608"/>
+        <c:axId val="305512832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2208,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256662144"/>
+        <c:crossAx val="305514368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2216,7 +2216,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256662144"/>
+        <c:axId val="305514368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2227,7 +2227,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256660608"/>
+        <c:crossAx val="305512832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2505,11 +2505,11 @@
         </c:dLbls>
         <c:gapWidth val="82"/>
         <c:overlap val="100"/>
-        <c:axId val="256115840"/>
-        <c:axId val="256117376"/>
+        <c:axId val="304697728"/>
+        <c:axId val="304699264"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256115840"/>
+        <c:axId val="304697728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2528,7 +2528,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="256117376"/>
+        <c:crossAx val="304699264"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2536,7 +2536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256117376"/>
+        <c:axId val="304699264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2547,7 +2547,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256115840"/>
+        <c:crossAx val="304697728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2802,11 +2802,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="32"/>
-        <c:axId val="256151552"/>
-        <c:axId val="256153088"/>
+        <c:axId val="304733184"/>
+        <c:axId val="304734976"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="256151552"/>
+        <c:axId val="304733184"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2815,7 +2815,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256153088"/>
+        <c:crossAx val="304734976"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2823,7 +2823,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="256153088"/>
+        <c:axId val="304734976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2834,7 +2834,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="in"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="256151552"/>
+        <c:crossAx val="304733184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="1"/>
@@ -3754,7 +3754,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3780,7 +3780,7 @@
         <v>55000</v>
       </c>
       <c r="C2" s="17">
-        <v>73100</v>
+        <v>74500</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -3883,7 +3883,7 @@
       </c>
       <c r="C8" s="17">
         <f>SUM(C2:C7)</f>
-        <v>95340</v>
+        <v>96740</v>
       </c>
       <c r="D8">
         <v>17</v>
@@ -3909,8 +3909,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3936,7 +3936,7 @@
         <v>55000</v>
       </c>
       <c r="C2" s="16">
-        <v>75800</v>
+        <v>78000</v>
       </c>
       <c r="D2">
         <v>8</v>
@@ -4021,7 +4021,7 @@
       </c>
       <c r="C7" s="16">
         <f>SUM(C2:C6)</f>
-        <v>105296</v>
+        <v>107496</v>
       </c>
       <c r="D7">
         <v>0.23</v>
@@ -4056,8 +4056,8 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A17:AG40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="AA20" sqref="AA20"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="4.125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>